<commit_message>
figure and data update
</commit_message>
<xml_diff>
--- a/Data/Modeling/BHE_Data.xlsx
+++ b/Data/Modeling/BHE_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4710" windowHeight="3345" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4716" windowHeight="3348" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="138">
   <si>
     <t>average energy consumption for a household</t>
   </si>
@@ -384,6 +384,63 @@
   <si>
     <t>for Q=1000W</t>
   </si>
+  <si>
+    <t>T (z alpha)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho c </t>
+  </si>
+  <si>
+    <t>V=pi x r2 x H</t>
+  </si>
+  <si>
+    <t>geoth. Recharge</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>Extraction</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>Vertical recharge</t>
+  </si>
+  <si>
+    <t>geother only account for</t>
+  </si>
+  <si>
+    <t>% of recharge</t>
+  </si>
+  <si>
+    <t>If unsteady state</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>% recharge</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>Lateral recharge</t>
+  </si>
+  <si>
+    <t>Q =rho c V DT</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>at 4.8 m</t>
+  </si>
+  <si>
+    <t>Unsteady state increase the share of vertical recharge</t>
+  </si>
 </sst>
 </file>
 
@@ -467,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,6 +539,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8606,17 +8665,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>34</v>
       </c>
@@ -8627,7 +8686,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8662,7 +8721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3">
         <f>B2*1000*3600</f>
         <v>44640000000</v>
@@ -8688,7 +8747,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -8729,7 +8788,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -8759,7 +8818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -8784,7 +8843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -8817,7 +8876,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I8" t="s">
         <v>23</v>
       </c>
@@ -8836,7 +8895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -8870,7 +8929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
         <v>26</v>
       </c>
@@ -8891,7 +8950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I11" t="s">
         <v>28</v>
       </c>
@@ -8902,7 +8961,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>44</v>
       </c>
@@ -8929,7 +8988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>45</v>
       </c>
@@ -8938,17 +8997,17 @@
       </c>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>47</v>
       </c>
@@ -8960,7 +9019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -8972,7 +9031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -8981,7 +9040,7 @@
         <v>199.83883964544722</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -8992,7 +9051,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -9003,7 +9062,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -9018,7 +9077,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B23">
         <f>C16/(80-40)</f>
         <v>24.979854955680903</v>
@@ -9030,7 +9089,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R29">
         <f>25*40</f>
         <v>1000</v>
@@ -9049,15 +9108,15 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>30</v>
       </c>
@@ -9074,7 +9133,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -9101,7 +9160,7 @@
         <v>31557599999.999973</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -9118,7 +9177,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -9145,7 +9204,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -9169,7 +9228,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -9196,7 +9255,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -9217,7 +9276,7 @@
         <v>-1293.4206780313489</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -9238,7 +9297,7 @@
         <v>-1293.0288749807671</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -9259,7 +9318,7 @@
         <v>-1292.5502411504472</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -9280,7 +9339,7 @@
         <v>-1291.9849183699239</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -9301,7 +9360,7 @@
         <v>-1291.3330741565364</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -9322,7 +9381,7 @@
         <v>-1290.5949016657933</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -9343,7 +9402,7 @@
         <v>-1289.7706196341355</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -9364,7 +9423,7 @@
         <v>-1288.8604723141179</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -9385,7 +9444,7 @@
         <v>-1287.8647294020338</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -9406,7 +9465,7 @@
         <v>-1286.7836859579984</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -9427,7 +9486,7 @@
         <v>-1285.6176623185147</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -9448,7 +9507,7 @@
         <v>-1284.3670040015522</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -9469,7 +9528,7 @@
         <v>-1283.0320816041615</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -9490,7 +9549,7 @@
         <v>-1281.6132906926587</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -9511,7 +9570,7 @@
         <v>-1280.111051685411</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -9532,7 +9591,7 @@
         <v>-1278.5258097282576</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -9553,7 +9612,7 @@
         <v>-1276.8580345626019</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -9574,7 +9633,7 @@
         <v>-1275.10822038622</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -9595,7 +9654,7 @@
         <v>-1273.2768857068161</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -9616,7 +9675,7 @@
         <v>-1271.3645731883787</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -9637,7 +9696,7 @@
         <v>-1269.3718494903785</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -9658,7 +9717,7 @@
         <v>-1267.2993050998537</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -9679,7 +9738,7 @@
         <v>-1265.1475541564364</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -9700,7 +9759,7 @@
         <v>-1262.9172342703698</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -9721,7 +9780,7 @@
         <v>-1260.6090063335701</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -9742,7 +9801,7 @@
         <v>-1258.2235543237907</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -9763,7 +9822,7 @@
         <v>-1255.7615851019441</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -9784,7 +9843,7 @@
         <v>-1253.2238282026453</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -9805,7 +9864,7 @@
         <v>-1250.6110356180322</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -9826,7 +9885,7 @@
         <v>-1247.9239815749361</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -9847,7 +9906,7 @@
         <v>-1245.163462305462</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -9868,7 +9927,7 @@
         <v>-1242.3302958110453</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -9889,7 +9948,7 @@
         <v>-1239.4253216200639</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -9910,7 +9969,7 @@
         <v>-1236.4494005390654</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -9931,7 +9990,7 @@
         <v>-1233.4034143976905</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -9952,7 +10011,7 @@
         <v>-1230.2882657873713</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -9973,7 +10032,7 @@
         <v>-1227.104877793872</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -9994,7 +10053,7 @@
         <v>-1223.8541937237571</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -10015,7 +10074,7 @@
         <v>-1220.5371768248731</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -10036,7 +10095,7 @@
         <v>-1217.1548100009136</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -10057,7 +10116,7 @@
         <v>-1213.7080955201664</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
@@ -10078,7 +10137,7 @@
         <v>-1210.1980547185176</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>46</v>
       </c>
@@ -10099,7 +10158,7 @@
         <v>-1206.6257276968108</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>47</v>
       </c>
@@ -10120,7 +10179,7 @@
         <v>-1202.9921730126389</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48</v>
       </c>
@@ -10141,7 +10200,7 @@
         <v>-1199.2984673666733</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
@@ -10162,7 +10221,7 @@
         <v>-1195.5457052836136</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>50</v>
       </c>
@@ -10183,7 +10242,7 @@
         <v>-1191.7349987878565</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>51</v>
       </c>
@@ -10204,7 +10263,7 @@
         <v>-1187.8674770739788</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>52</v>
       </c>
@@ -10225,7 +10284,7 @@
         <v>-1183.9442861721311</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>53</v>
       </c>
@@ -10246,7 +10305,7 @@
         <v>-1179.9665886084481</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>54</v>
       </c>
@@ -10267,7 +10326,7 @@
         <v>-1175.9355630605637</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>55</v>
       </c>
@@ -10288,7 +10347,7 @@
         <v>-1171.8524040083437</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>56</v>
       </c>
@@ -10309,7 +10368,7 @@
         <v>-1167.7183213799374</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>57</v>
       </c>
@@ -10330,7 +10389,7 @@
         <v>-1163.5345401932484</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>58</v>
       </c>
@@ -10351,7 +10410,7 @@
         <v>-1159.3023001929359</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>59</v>
       </c>
@@ -10372,7 +10431,7 @@
         <v>-1155.0228554830505</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>60</v>
       </c>
@@ -10393,7 +10452,7 @@
         <v>-1150.6974741554188</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>61</v>
       </c>
@@ -10414,7 +10473,7 @@
         <v>-1146.3274379138768</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>62</v>
       </c>
@@ -10435,7 +10494,7 @@
         <v>-1141.9140416944758</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>63</v>
       </c>
@@ -10456,7 +10515,7 @@
         <v>-1137.4585932817656</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>64</v>
       </c>
@@ -10477,7 +10536,7 @@
         <v>-1132.9624129212662</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>65</v>
       </c>
@@ -10498,7 +10557,7 @@
         <v>-1128.4268329282543</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>66</v>
       </c>
@@ -10519,7 +10578,7 @@
         <v>-1123.8531972929673</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>67</v>
       </c>
@@ -10540,7 +10599,7 @@
         <v>-1119.2428612823521</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>68</v>
       </c>
@@ -10561,7 +10620,7 @@
         <v>-1114.5971910384674</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>69</v>
       </c>
@@ -10582,7 +10641,7 @@
         <v>-1109.9175631736673</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>70</v>
       </c>
@@ -10603,7 +10662,7 @@
         <v>-1105.2053643626841</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>71</v>
       </c>
@@ -10624,7 +10683,7 @@
         <v>-1100.4619909317221</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>72</v>
       </c>
@@ -10645,7 +10704,7 @@
         <v>-1095.6888484446999</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>73</v>
       </c>
@@ -10666,7 +10725,7 @@
         <v>-1090.8873512867492</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>74</v>
       </c>
@@ -10687,7 +10746,7 @@
         <v>-1086.0589222451026</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>75</v>
       </c>
@@ -10708,7 +10767,7 @@
         <v>-1081.2049920874908</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>76</v>
       </c>
@@ -10729,7 +10788,7 @@
         <v>-1076.3269991381765</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>77</v>
       </c>
@@ -10750,7 +10809,7 @@
         <v>-1071.4263888517457</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>78</v>
       </c>
@@ -10771,7 +10830,7 @@
         <v>-1066.5046133847904</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>79</v>
       </c>
@@ -10792,7 +10851,7 @@
         <v>-1061.5631311656025</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>80</v>
       </c>
@@ -10813,7 +10872,7 @@
         <v>-1056.6034064620089</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>81</v>
       </c>
@@ -10834,7 +10893,7 @@
         <v>-1051.6269089474788</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>82</v>
       </c>
@@ -10855,7 +10914,7 @@
         <v>-1046.6351132656278</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>83</v>
       </c>
@@ -10876,7 +10935,7 @@
         <v>-1041.6294985932479</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>84</v>
       </c>
@@ -10897,7 +10956,7 @@
         <v>-1036.6115482019968</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>85</v>
       </c>
@@ -10918,7 +10977,7 @@
         <v>-1031.5827490188715</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>86</v>
       </c>
@@ -10939,7 +10998,7 @@
         <v>-1026.5445911856004</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>87</v>
       </c>
@@ -10960,7 +11019,7 @@
         <v>-1021.4985676170818</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>88</v>
       </c>
@@ -10981,7 +11040,7 @@
         <v>-1016.4461735590008</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>89</v>
       </c>
@@ -11002,7 +11061,7 @@
         <v>-1011.3889061447572</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>90</v>
       </c>
@@ -11023,7 +11082,7 @@
         <v>-1006.32826395183</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>91</v>
       </c>
@@ -11044,7 +11103,7 @@
         <v>-1001.2657465577189</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>92</v>
       </c>
@@ -11065,7 +11124,7 @@
         <v>-996.20285409558562</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>93</v>
       </c>
@@ -11086,7 +11145,7 @@
         <v>-991.14108680973277</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>94</v>
       </c>
@@ -11107,7 +11166,7 @@
         <v>-986.08194461104938</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>95</v>
       </c>
@@ -11128,7 +11187,7 @@
         <v>-981.02692663255414</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>96</v>
       </c>
@@ -11149,7 +11208,7 @@
         <v>-975.97753078516985</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>97</v>
       </c>
@@ -11170,7 +11229,7 @@
         <v>-970.93525331386127</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>98</v>
       </c>
@@ -11191,7 +11250,7 @@
         <v>-965.9015883542645</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>99</v>
       </c>
@@ -11212,7 +11271,7 @@
         <v>-960.8780274899425</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>100</v>
       </c>
@@ -11233,7 +11292,7 @@
         <v>-955.86605931039639</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>101</v>
       </c>
@@ -11254,7 +11313,7 @@
         <v>-950.86716896996495</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>102</v>
       </c>
@@ -11275,7 +11334,7 @@
         <v>-945.88283774774106</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>103</v>
       </c>
@@ -11296,7 +11355,7 @@
         <v>-940.91454260863657</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>104</v>
       </c>
@@ -11317,7 +11376,7 @@
         <v>-935.96375576572609</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>105</v>
       </c>
@@ -11338,7 +11397,7 @@
         <v>-931.03194424399726</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>106</v>
       </c>
@@ -11359,7 +11418,7 @@
         <v>-926.12056944564154</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>107</v>
       </c>
@@ -11380,7 +11439,7 @@
         <v>-921.23108671700788</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>108</v>
       </c>
@@ -11401,7 +11460,7 @@
         <v>-916.36494491735198</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>109</v>
       </c>
@@ -11422,7 +11481,7 @@
         <v>-911.52358598950946</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>110</v>
       </c>
@@ -11443,7 +11502,7 @@
         <v>-906.70844453261589</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>111</v>
       </c>
@@ -11464,7 +11523,7 @@
         <v>-901.92094737700381</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>112</v>
       </c>
@@ -11485,7 +11544,7 @@
         <v>-897.16251316140347</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>113</v>
       </c>
@@ -11506,7 +11565,7 @@
         <v>-892.43455191256794</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>114</v>
       </c>
@@ -11527,7 +11586,7 @@
         <v>-887.73846462745337</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>115</v>
       </c>
@@ -11548,7 +11607,7 @@
         <v>-883.07564285807189</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>116</v>
       </c>
@@ -11569,7 +11628,7 @@
         <v>-878.44746829914607</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>117</v>
       </c>
@@ -11590,7 +11649,7 @@
         <v>-873.85531237868122</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>118</v>
       </c>
@@ -11611,7 +11670,7 @@
         <v>-869.3005358515843</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>119</v>
       </c>
@@ -11632,7 +11691,7 @@
         <v>-864.78448839644</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>120</v>
       </c>
@@ -11653,7 +11712,7 @@
         <v>-860.30850821557374</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>121</v>
       </c>
@@ -11674,7 +11733,7 @@
         <v>-855.873921638512</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>122</v>
       </c>
@@ -11695,7 +11754,7 @@
         <v>-851.48204272896464</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>123</v>
       </c>
@@ -11716,7 +11775,7 @@
         <v>-847.13417289543645</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>124</v>
       </c>
@@ -11737,7 +11796,7 @@
         <v>-842.83160050559445</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>125</v>
       </c>
@@ -11758,7 +11817,7 @@
         <v>-838.57560050449433</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>126</v>
       </c>
@@ -11779,7 +11838,7 @@
         <v>-834.3674340367885</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>127</v>
       </c>
@@ -11800,7 +11859,7 @@
         <v>-830.2083480730214</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>128</v>
       </c>
@@ -11821,7 +11880,7 @@
         <v>-826.09957504012391</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>129</v>
       </c>
@@ -11842,7 +11901,7 @@
         <v>-822.04233245622095</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>130</v>
       </c>
@@ -11863,7 +11922,7 @@
         <v>-818.03782256985198</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>131</v>
       </c>
@@ -11884,7 +11943,7 @@
         <v>-814.08723200372106</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>132</v>
       </c>
@@ -11905,7 +11964,7 @@
         <v>-810.19173140307362</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>133</v>
       </c>
@@ -11926,7 +11985,7 @@
         <v>-806.352475088809</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>134</v>
       </c>
@@ -11947,7 +12006,7 @@
         <v>-802.57060071543196</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>135</v>
       </c>
@@ -11968,7 +12027,7 @@
         <v>-798.84722893393825</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>136</v>
       </c>
@@ -11989,7 +12048,7 @@
         <v>-795.18346305974342</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>137</v>
       </c>
@@ -12010,7 +12069,7 @@
         <v>-791.58038874574709</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>138</v>
       </c>
@@ -12031,7 +12090,7 @@
         <v>-788.03907366062924</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>139</v>
       </c>
@@ -12052,7 +12111,7 @@
         <v>-784.56056717247702</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>140</v>
       </c>
@@ -12073,7 +12132,7 @@
         <v>-781.14590003783519</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>141</v>
       </c>
@@ -12094,7 +12153,7 @@
         <v>-777.79608409627053</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>142</v>
       </c>
@@ -12115,7 +12174,7 @@
         <v>-774.51211197054158</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>143</v>
       </c>
@@ -12136,7 +12195,7 @@
         <v>-771.29495677246291</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>144</v>
       </c>
@@ -12157,7 +12216,7 @@
         <v>-768.1455718145512</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>145</v>
       </c>
@@ -12178,7 +12237,7 @@
         <v>-765.06489032753984</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>146</v>
       </c>
@@ -12199,7 +12258,7 @@
         <v>-762.05382518383908</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>147</v>
       </c>
@@ -12220,7 +12279,7 @@
         <v>-759.11326862703527</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>148</v>
       </c>
@@ -12241,7 +12300,7 @@
         <v>-756.24409200749892</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>149</v>
       </c>
@@ -12262,7 +12321,7 @@
         <v>-753.44714552418407</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>150</v>
       </c>
@@ -12283,7 +12342,7 @@
         <v>-750.72325797269696</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>151</v>
       </c>
@@ -12304,7 +12363,7 @@
         <v>-748.07323649970476</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>152</v>
       </c>
@@ -12325,7 +12384,7 @@
         <v>-745.49786636376302</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>153</v>
       </c>
@@ -12346,7 +12405,7 @@
         <v>-742.99791070262336</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>154</v>
       </c>
@@ -12367,7 +12426,7 @@
         <v>-740.57411030710205</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>155</v>
       </c>
@@ -12388,7 +12447,7 @@
         <v>-738.22718340156575</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>156</v>
       </c>
@@ -12409,7 +12468,7 @@
         <v>-735.95782543110772</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>157</v>
       </c>
@@ -12430,7 +12489,7 @@
         <v>-733.76670885547128</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>158</v>
       </c>
@@ -12451,7 +12510,7 @@
         <v>-731.65448294978614</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>159</v>
       </c>
@@ -12472,7 +12531,7 @@
         <v>-729.62177361217357</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>160</v>
       </c>
@@ -12493,7 +12552,7 @@
         <v>-727.66918317827958</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>161</v>
       </c>
@@ -12514,7 +12573,7 @@
         <v>-725.79729024279015</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>162</v>
       </c>
@@ -12535,7 +12594,7 @@
         <v>-724.00664948798112</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>163</v>
       </c>
@@ -12556,7 +12615,7 @@
         <v>-722.29779151935315</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>164</v>
       </c>
@@ -12577,7 +12636,7 @@
         <v>-720.67122270840264</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>165</v>
       </c>
@@ -12598,7 +12657,7 @@
         <v>-719.12742504257199</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>166</v>
       </c>
@@ -12619,7 +12678,7 @@
         <v>-717.66685598242805</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>167</v>
       </c>
@@ -12640,7 +12699,7 @@
         <v>-716.28994832610488</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>168</v>
       </c>
@@ -12661,7 +12720,7 @@
         <v>-714.99711008105714</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>169</v>
       </c>
@@ -12682,7 +12741,7 @@
         <v>-713.78872434315838</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>170</v>
       </c>
@@ -12703,7 +12762,7 @@
         <v>-712.66514918318194</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>171</v>
       </c>
@@ -12724,7 +12783,7 @@
         <v>-711.62671754069652</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>172</v>
       </c>
@@ -12745,7 +12804,7 @@
         <v>-710.67373712540893</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>173</v>
       </c>
@@ -12766,7 +12825,7 @@
         <v>-709.80649032598319</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>174</v>
       </c>
@@ -12787,7 +12846,7 @@
         <v>-709.02523412636276</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>175</v>
       </c>
@@ -12808,7 +12867,7 @@
         <v>-708.33020002962064</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>176</v>
       </c>
@@ -12829,7 +12888,7 @@
         <v>-707.72159398935946</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>177</v>
       </c>
@@ -12850,7 +12909,7 @@
         <v>-707.19959634868383</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>178</v>
       </c>
@@ -12871,7 +12930,7 @@
         <v>-706.76436178676033</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>179</v>
       </c>
@@ -12892,7 +12951,7 @@
         <v>-706.41601927298279</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>180</v>
       </c>
@@ -12913,7 +12972,7 @@
         <v>-706.15467202875595</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>181</v>
       </c>
@@ -12934,7 +12993,7 @@
         <v>-705.98039749690849</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>182</v>
       </c>
@@ -12955,7 +13014,7 @@
         <v>-705.89324731874558</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>183</v>
       </c>
@@ -12976,7 +13035,7 @@
         <v>-705.89324731874558</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>184</v>
       </c>
@@ -12997,7 +13056,7 @@
         <v>-705.98039749690849</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>185</v>
       </c>
@@ -13018,7 +13077,7 @@
         <v>-706.15467202875595</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>186</v>
       </c>
@@ -13039,7 +13098,7 @@
         <v>-706.41601927298279</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>187</v>
       </c>
@@ -13060,7 +13119,7 @@
         <v>-706.76436178676033</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>188</v>
       </c>
@@ -13081,7 +13140,7 @@
         <v>-707.19959634868383</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>189</v>
       </c>
@@ -13102,7 +13161,7 @@
         <v>-707.72159398935923</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>190</v>
       </c>
@@ -13123,7 +13182,7 @@
         <v>-708.33020002962064</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>191</v>
       </c>
@@ -13144,7 +13203,7 @@
         <v>-709.02523412636276</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>192</v>
       </c>
@@ -13165,7 +13224,7 @@
         <v>-709.80649032598319</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>193</v>
       </c>
@@ -13186,7 +13245,7 @@
         <v>-710.67373712540871</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>194</v>
       </c>
@@ -13207,7 +13266,7 @@
         <v>-711.62671754069652</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>195</v>
       </c>
@@ -13228,7 +13287,7 @@
         <v>-712.66514918318194</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>196</v>
       </c>
@@ -13249,7 +13308,7 @@
         <v>-713.78872434315826</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>197</v>
       </c>
@@ -13270,7 +13329,7 @@
         <v>-714.99711008105692</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>198</v>
       </c>
@@ -13291,7 +13350,7 @@
         <v>-716.28994832610488</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>199</v>
       </c>
@@ -13312,7 +13371,7 @@
         <v>-717.66685598242805</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>200</v>
       </c>
@@ -13333,7 +13392,7 @@
         <v>-719.12742504257199</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>201</v>
       </c>
@@ -13354,7 +13413,7 @@
         <v>-720.67122270840252</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>202</v>
       </c>
@@ -13375,7 +13434,7 @@
         <v>-722.29779151935315</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>203</v>
       </c>
@@ -13396,7 +13455,7 @@
         <v>-724.00664948798101</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>204</v>
       </c>
@@ -13417,7 +13476,7 @@
         <v>-725.79729024279015</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>205</v>
       </c>
@@ -13438,7 +13497,7 @@
         <v>-727.66918317827958</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>206</v>
       </c>
@@ -13459,7 +13518,7 @@
         <v>-729.62177361217346</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>207</v>
       </c>
@@ -13480,7 +13539,7 @@
         <v>-731.65448294978614</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>208</v>
       </c>
@@ -13501,7 +13560,7 @@
         <v>-733.76670885547128</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>209</v>
       </c>
@@ -13522,7 +13581,7 @@
         <v>-735.95782543110772</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>210</v>
       </c>
@@ -13543,7 +13602,7 @@
         <v>-738.22718340156575</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>211</v>
       </c>
@@ -13564,7 +13623,7 @@
         <v>-740.57411030710205</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>212</v>
       </c>
@@ -13585,7 +13644,7 @@
         <v>-742.99791070262324</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>213</v>
       </c>
@@ -13606,7 +13665,7 @@
         <v>-745.49786636376291</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>214</v>
       </c>
@@ -13627,7 +13686,7 @@
         <v>-748.07323649970476</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>215</v>
       </c>
@@ -13648,7 +13707,7 @@
         <v>-750.72325797269673</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>216</v>
       </c>
@@ -13669,7 +13728,7 @@
         <v>-753.44714552418407</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>217</v>
       </c>
@@ -13690,7 +13749,7 @@
         <v>-756.24409200749892</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>218</v>
       </c>
@@ -13711,7 +13770,7 @@
         <v>-759.11326862703527</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>219</v>
       </c>
@@ -13732,7 +13791,7 @@
         <v>-762.05382518383874</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>220</v>
       </c>
@@ -13753,7 +13812,7 @@
         <v>-765.06489032753962</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>221</v>
       </c>
@@ -13774,7 +13833,7 @@
         <v>-768.1455718145512</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>222</v>
       </c>
@@ -13795,7 +13854,7 @@
         <v>-771.29495677246268</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>223</v>
       </c>
@@ -13816,7 +13875,7 @@
         <v>-774.51211197054135</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>224</v>
       </c>
@@ -13837,7 +13896,7 @@
         <v>-777.79608409627053</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>225</v>
       </c>
@@ -13858,7 +13917,7 @@
         <v>-781.14590003783496</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>226</v>
       </c>
@@ -13879,7 +13938,7 @@
         <v>-784.56056717247657</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>227</v>
       </c>
@@ -13900,7 +13959,7 @@
         <v>-788.0390736606289</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>228</v>
       </c>
@@ -13921,7 +13980,7 @@
         <v>-791.58038874574709</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>229</v>
       </c>
@@ -13942,7 +14001,7 @@
         <v>-795.18346305974342</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>230</v>
       </c>
@@ -13963,7 +14022,7 @@
         <v>-798.84722893393814</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>231</v>
       </c>
@@ -13984,7 +14043,7 @@
         <v>-802.57060071543174</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>232</v>
       </c>
@@ -14005,7 +14064,7 @@
         <v>-806.352475088809</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>233</v>
       </c>
@@ -14026,7 +14085,7 @@
         <v>-810.19173140307316</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>234</v>
       </c>
@@ -14047,7 +14106,7 @@
         <v>-814.08723200372106</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>235</v>
       </c>
@@ -14068,7 +14127,7 @@
         <v>-818.03782256985187</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>236</v>
       </c>
@@ -14089,7 +14148,7 @@
         <v>-822.04233245622061</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>237</v>
       </c>
@@ -14110,7 +14169,7 @@
         <v>-826.09957504012391</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>238</v>
       </c>
@@ -14131,7 +14190,7 @@
         <v>-830.2083480730214</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>239</v>
       </c>
@@ -14152,7 +14211,7 @@
         <v>-834.3674340367885</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>240</v>
       </c>
@@ -14173,7 +14232,7 @@
         <v>-838.5756005044941</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>241</v>
       </c>
@@ -14194,7 +14253,7 @@
         <v>-842.83160050559434</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>242</v>
       </c>
@@ -14215,7 +14274,7 @@
         <v>-847.13417289543645</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>243</v>
       </c>
@@ -14236,7 +14295,7 @@
         <v>-851.48204272896442</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>244</v>
       </c>
@@ -14257,7 +14316,7 @@
         <v>-855.873921638512</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>245</v>
       </c>
@@ -14278,7 +14337,7 @@
         <v>-860.30850821557328</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>246</v>
       </c>
@@ -14299,7 +14358,7 @@
         <v>-864.78448839643988</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>247</v>
       </c>
@@ -14320,7 +14379,7 @@
         <v>-869.3005358515843</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>248</v>
       </c>
@@ -14341,7 +14400,7 @@
         <v>-873.85531237868099</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>249</v>
       </c>
@@ -14362,7 +14421,7 @@
         <v>-878.44746829914573</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>250</v>
       </c>
@@ -14383,7 +14442,7 @@
         <v>-883.07564285807166</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>251</v>
       </c>
@@ -14404,7 +14463,7 @@
         <v>-887.73846462745314</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>252</v>
       </c>
@@ -14425,7 +14484,7 @@
         <v>-892.43455191256794</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>253</v>
       </c>
@@ -14446,7 +14505,7 @@
         <v>-897.16251316140324</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>254</v>
       </c>
@@ -14467,7 +14526,7 @@
         <v>-901.9209473770037</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>255</v>
       </c>
@@ -14488,7 +14547,7 @@
         <v>-906.70844453261554</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>256</v>
       </c>
@@ -14509,7 +14568,7 @@
         <v>-911.52358598950946</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>257</v>
       </c>
@@ -14530,7 +14589,7 @@
         <v>-916.36494491735175</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>258</v>
       </c>
@@ -14551,7 +14610,7 @@
         <v>-921.23108671700743</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>259</v>
       </c>
@@ -14572,7 +14631,7 @@
         <v>-926.12056944564119</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>260</v>
       </c>
@@ -14593,7 +14652,7 @@
         <v>-931.03194424399692</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>261</v>
       </c>
@@ -14614,7 +14673,7 @@
         <v>-935.96375576572564</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>262</v>
       </c>
@@ -14635,7 +14694,7 @@
         <v>-940.91454260863657</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>263</v>
       </c>
@@ -14656,7 +14715,7 @@
         <v>-945.88283774774095</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>264</v>
       </c>
@@ -14677,7 +14736,7 @@
         <v>-950.86716896996472</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>265</v>
       </c>
@@ -14698,7 +14757,7 @@
         <v>-955.86605931039594</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>266</v>
       </c>
@@ -14719,7 +14778,7 @@
         <v>-960.87802748994227</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>267</v>
       </c>
@@ -14740,7 +14799,7 @@
         <v>-965.9015883542645</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>268</v>
       </c>
@@ -14761,7 +14820,7 @@
         <v>-970.93525331386104</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>269</v>
       </c>
@@ -14782,7 +14841,7 @@
         <v>-975.97753078516962</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>270</v>
       </c>
@@ -14803,7 +14862,7 @@
         <v>-981.02692663255402</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>271</v>
       </c>
@@ -14824,7 +14883,7 @@
         <v>-986.08194461104927</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>272</v>
       </c>
@@ -14845,7 +14904,7 @@
         <v>-991.14108680973277</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>273</v>
       </c>
@@ -14866,7 +14925,7 @@
         <v>-996.20285409558528</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>274</v>
       </c>
@@ -14887,7 +14946,7 @@
         <v>-1001.2657465577186</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>275</v>
       </c>
@@ -14908,7 +14967,7 @@
         <v>-1006.3282639518296</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>276</v>
       </c>
@@ -14929,7 +14988,7 @@
         <v>-1011.3889061447571</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>277</v>
       </c>
@@ -14950,7 +15009,7 @@
         <v>-1016.4461735590008</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>278</v>
       </c>
@@ -14971,7 +15030,7 @@
         <v>-1021.4985676170813</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>279</v>
       </c>
@@ -14992,7 +15051,7 @@
         <v>-1026.5445911856002</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>280</v>
       </c>
@@ -15013,7 +15072,7 @@
         <v>-1031.5827490188713</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>281</v>
       </c>
@@ -15034,7 +15093,7 @@
         <v>-1036.6115482019966</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>282</v>
       </c>
@@ -15055,7 +15114,7 @@
         <v>-1041.6294985932479</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>283</v>
       </c>
@@ -15076,7 +15135,7 @@
         <v>-1046.6351132656275</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>284</v>
       </c>
@@ -15097,7 +15156,7 @@
         <v>-1051.6269089474788</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>285</v>
       </c>
@@ -15118,7 +15177,7 @@
         <v>-1056.6034064620085</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>286</v>
       </c>
@@ -15139,7 +15198,7 @@
         <v>-1061.5631311656025</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>287</v>
       </c>
@@ -15160,7 +15219,7 @@
         <v>-1066.5046133847904</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>288</v>
       </c>
@@ -15181,7 +15240,7 @@
         <v>-1071.4263888517455</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>289</v>
       </c>
@@ -15202,7 +15261,7 @@
         <v>-1076.3269991381762</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>290</v>
       </c>
@@ -15223,7 +15282,7 @@
         <v>-1081.2049920874904</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>291</v>
       </c>
@@ -15244,7 +15303,7 @@
         <v>-1086.0589222451024</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>292</v>
       </c>
@@ -15265,7 +15324,7 @@
         <v>-1090.8873512867492</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>293</v>
       </c>
@@ -15286,7 +15345,7 @@
         <v>-1095.6888484446999</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>294</v>
       </c>
@@ -15307,7 +15366,7 @@
         <v>-1100.4619909317219</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>295</v>
       </c>
@@ -15328,7 +15387,7 @@
         <v>-1105.2053643626837</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>296</v>
       </c>
@@ -15349,7 +15408,7 @@
         <v>-1109.9175631736668</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>297</v>
       </c>
@@ -15370,7 +15429,7 @@
         <v>-1114.5971910384669</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>298</v>
       </c>
@@ -15391,7 +15450,7 @@
         <v>-1119.2428612823521</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>299</v>
       </c>
@@ -15412,7 +15471,7 @@
         <v>-1123.8531972929673</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>300</v>
       </c>
@@ -15433,7 +15492,7 @@
         <v>-1128.4268329282538</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>301</v>
       </c>
@@ -15454,7 +15513,7 @@
         <v>-1132.9624129212659</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>302</v>
       </c>
@@ -15475,7 +15534,7 @@
         <v>-1137.4585932817654</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>303</v>
       </c>
@@ -15496,7 +15555,7 @@
         <v>-1141.9140416944758</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>304</v>
       </c>
@@ -15517,7 +15576,7 @@
         <v>-1146.3274379138766</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>305</v>
       </c>
@@ -15538,7 +15597,7 @@
         <v>-1150.6974741554184</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>306</v>
       </c>
@@ -15559,7 +15618,7 @@
         <v>-1155.0228554830503</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>307</v>
       </c>
@@ -15580,7 +15639,7 @@
         <v>-1159.3023001929355</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>308</v>
       </c>
@@ -15601,7 +15660,7 @@
         <v>-1163.5345401932482</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>309</v>
       </c>
@@ -15622,7 +15681,7 @@
         <v>-1167.7183213799374</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>310</v>
       </c>
@@ -15643,7 +15702,7 @@
         <v>-1171.8524040083435</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>311</v>
       </c>
@@ -15664,7 +15723,7 @@
         <v>-1175.9355630605633</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>312</v>
       </c>
@@ -15685,7 +15744,7 @@
         <v>-1179.9665886084481</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>313</v>
       </c>
@@ -15706,7 +15765,7 @@
         <v>-1183.9442861721309</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>314</v>
       </c>
@@ -15727,7 +15786,7 @@
         <v>-1187.8674770739783</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>315</v>
       </c>
@@ -15748,7 +15807,7 @@
         <v>-1191.7349987878563</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>316</v>
       </c>
@@ -15769,7 +15828,7 @@
         <v>-1195.5457052836134</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>317</v>
       </c>
@@ -15790,7 +15849,7 @@
         <v>-1199.2984673666733</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>318</v>
       </c>
@@ -15811,7 +15870,7 @@
         <v>-1202.9921730126387</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>319</v>
       </c>
@@ -15832,7 +15891,7 @@
         <v>-1206.6257276968108</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>320</v>
       </c>
@@ -15853,7 +15912,7 @@
         <v>-1210.1980547185176</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>321</v>
       </c>
@@ -15874,7 +15933,7 @@
         <v>-1213.7080955201664</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>322</v>
       </c>
@@ -15895,7 +15954,7 @@
         <v>-1217.1548100009136</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>323</v>
       </c>
@@ -15916,7 +15975,7 @@
         <v>-1220.5371768248731</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>324</v>
       </c>
@@ -15937,7 +15996,7 @@
         <v>-1223.8541937237571</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>325</v>
       </c>
@@ -15958,7 +16017,7 @@
         <v>-1227.104877793872</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>326</v>
       </c>
@@ -15979,7 +16038,7 @@
         <v>-1230.2882657873713</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>327</v>
       </c>
@@ -16000,7 +16059,7 @@
         <v>-1233.4034143976903</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>328</v>
       </c>
@@ -16021,7 +16080,7 @@
         <v>-1236.4494005390652</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>329</v>
       </c>
@@ -16042,7 +16101,7 @@
         <v>-1239.4253216200639</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>330</v>
       </c>
@@ -16063,7 +16122,7 @@
         <v>-1242.3302958110453</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>331</v>
       </c>
@@ -16084,7 +16143,7 @@
         <v>-1245.1634623054617</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>332</v>
       </c>
@@ -16105,7 +16164,7 @@
         <v>-1247.9239815749361</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>333</v>
       </c>
@@ -16126,7 +16185,7 @@
         <v>-1250.611035618032</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>334</v>
       </c>
@@ -16147,7 +16206,7 @@
         <v>-1253.2238282026453</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>335</v>
       </c>
@@ -16168,7 +16227,7 @@
         <v>-1255.7615851019441</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>336</v>
       </c>
@@ -16189,7 +16248,7 @@
         <v>-1258.2235543237907</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>337</v>
       </c>
@@ -16210,7 +16269,7 @@
         <v>-1260.6090063335701</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>338</v>
       </c>
@@ -16231,7 +16290,7 @@
         <v>-1262.9172342703696</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>339</v>
       </c>
@@ -16252,7 +16311,7 @@
         <v>-1265.1475541564364</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>340</v>
       </c>
@@ -16273,7 +16332,7 @@
         <v>-1267.2993050998537</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>341</v>
       </c>
@@ -16294,7 +16353,7 @@
         <v>-1269.3718494903783</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>342</v>
       </c>
@@ -16315,7 +16374,7 @@
         <v>-1271.3645731883787</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>343</v>
       </c>
@@ -16336,7 +16395,7 @@
         <v>-1273.2768857068158</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>344</v>
       </c>
@@ -16357,7 +16416,7 @@
         <v>-1275.10822038622</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>345</v>
       </c>
@@ -16378,7 +16437,7 @@
         <v>-1276.8580345626019</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>346</v>
       </c>
@@ -16399,7 +16458,7 @@
         <v>-1278.5258097282576</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>347</v>
       </c>
@@ -16420,7 +16479,7 @@
         <v>-1280.111051685411</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>348</v>
       </c>
@@ -16441,7 +16500,7 @@
         <v>-1281.6132906926584</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>349</v>
       </c>
@@ -16462,7 +16521,7 @@
         <v>-1283.0320816041612</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>350</v>
       </c>
@@ -16483,7 +16542,7 @@
         <v>-1284.3670040015522</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>351</v>
       </c>
@@ -16504,7 +16563,7 @@
         <v>-1285.6176623185147</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>352</v>
       </c>
@@ -16525,7 +16584,7 @@
         <v>-1286.7836859579984</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>353</v>
       </c>
@@ -16546,7 +16605,7 @@
         <v>-1287.8647294020338</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>354</v>
       </c>
@@ -16567,7 +16626,7 @@
         <v>-1288.8604723141179</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>355</v>
       </c>
@@ -16588,7 +16647,7 @@
         <v>-1289.7706196341355</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>356</v>
       </c>
@@ -16609,7 +16668,7 @@
         <v>-1290.5949016657933</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>357</v>
       </c>
@@ -16630,7 +16689,7 @@
         <v>-1291.3330741565364</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>358</v>
       </c>
@@ -16651,7 +16710,7 @@
         <v>-1291.9849183699239</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>359</v>
       </c>
@@ -16672,7 +16731,7 @@
         <v>-1292.5502411504472</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>360</v>
       </c>
@@ -16693,7 +16752,7 @@
         <v>-1293.0288749807671</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>361</v>
       </c>
@@ -16714,7 +16773,7 @@
         <v>-1293.4206780313489</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>362</v>
       </c>
@@ -16735,7 +16794,7 @@
         <v>-1293.7255342024928</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>363</v>
       </c>
@@ -16756,7 +16815,7 @@
         <v>-1293.9433531587367</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>364</v>
       </c>
@@ -16777,7 +16836,7 @@
         <v>-1294.0740703556226</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>365</v>
       </c>
@@ -16798,13 +16857,13 @@
         <v>-1294.1176470588234</v>
       </c>
     </row>
-    <row r="370" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="370" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M370">
         <f>MIN(M4:M368)</f>
         <v>-1294.1176470588234</v>
       </c>
     </row>
-    <row r="371" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="371" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M371">
         <f>MAX(M4:M368)</f>
         <v>-705.89324731874558</v>
@@ -16818,19 +16877,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -16851,7 +16910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -16881,7 +16940,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -16895,10 +16954,12 @@
         <v>76</v>
       </c>
       <c r="I3" s="7">
-        <f>I7/((1-I5)*I4*I6*I1*I2)</f>
+        <f>I7/(I4*I6*I1*I2 * (1-I5))</f>
         <v>6803.5896192093132</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="M3">
         <v>1415</v>
       </c>
@@ -16912,7 +16973,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -16930,7 +16991,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -16949,7 +17010,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -16972,7 +17033,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -16993,7 +17054,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -17010,7 +17071,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -17019,7 +17080,7 @@
         <v>31532170829.975826</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -17033,8 +17094,14 @@
         <v>5</v>
       </c>
       <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="12">
+        <v>31500000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>76</v>
       </c>
@@ -17049,12 +17116,19 @@
         <v>76</v>
       </c>
       <c r="I11" s="10">
-        <f>I7/(I10*(1-I5)*I1*I2)</f>
+        <f>I7/(I10*I1*I2*(1-I5))</f>
         <v>2952.757894736842</v>
       </c>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O11" s="12">
+        <f>70*0.031</f>
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>100</v>
       </c>
@@ -17065,8 +17139,15 @@
       <c r="C12" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="O12" s="12">
+        <f>950*2500</f>
+        <v>2375000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H13" s="5" t="s">
         <v>109</v>
       </c>
@@ -17074,8 +17155,15 @@
         <v>110</v>
       </c>
       <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="13">
+        <f>O10/(O11*O12)</f>
+        <v>6112.0543293718165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>78</v>
       </c>
@@ -17086,8 +17174,14 @@
         <v>40</v>
       </c>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -17105,8 +17199,12 @@
         <v>7.3580735205142798</v>
       </c>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -17131,8 +17229,22 @@
         <v>4.8474014414992848</v>
       </c>
       <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>6.4736000000000002E-2</v>
+      </c>
+      <c r="L16">
+        <f>K16*I18</f>
+        <v>4.7787433768421064</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="O16" s="5">
+        <f>SQRT(O13/(PI()*O14))</f>
+        <v>6.9741080396196331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -17158,9 +17270,19 @@
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="5">
+        <f>B8-L16</f>
+        <v>994.41545485039387</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="5">
+        <f>O16^2*PI()</f>
+        <v>152.80135823429541</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>86</v>
       </c>
@@ -17176,10 +17298,18 @@
         <v>73.818947368421064</v>
       </c>
       <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L18">
+        <f>L17/(B15)</f>
+        <v>24.860386371259846</v>
+      </c>
+      <c r="M18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>101</v>
       </c>
@@ -17187,24 +17317,39 @@
         <f>PI()*B17^2</f>
         <v>2087.5319980123022</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19">
+        <f>2*PI()*I16</f>
+        <v>30.457121515229453</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="H20" s="11" t="s">
         <v>83</v>
       </c>
       <c r="I20" s="11">
-        <f>1000/(K21+K22)</f>
-        <v>5813.9534883720935</v>
+        <f>1000/(K23+K24)</f>
+        <v>5821.5350223546939</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>94</v>
+      </c>
+      <c r="L20">
+        <f>L18/L19</f>
+        <v>0.81624215075048789</v>
+      </c>
+      <c r="M20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>83</v>
       </c>
@@ -17218,33 +17363,19 @@
       <c r="J21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="11">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="L21" s="5">
-        <f>I17*K22</f>
-        <v>13.607179238418626</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>87</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5">
         <f>I20/I21</f>
-        <v>34.181682398696871</v>
+        <v>34.226256127607243</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="11">
-        <v>0.08</v>
-      </c>
-      <c r="L22" s="5">
-        <f>I18*K22</f>
-        <v>5.9055157894736849</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -17254,13 +17385,16 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="K23" s="11">
+        <f>0.091923</f>
+        <v>9.1923000000000005E-2</v>
+      </c>
       <c r="L23" s="5">
-        <f>1000-(L21+L22)</f>
-        <v>980.48730497210772</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <f>I18*K23</f>
+        <v>6.7856590989473702</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -17270,15 +17404,16 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="L24" s="8">
-        <f>2*PI()*I16</f>
-        <v>30.457121515229453</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K24" s="11">
+        <f>K23-0.01207</f>
+        <v>7.9853000000000007E-2</v>
+      </c>
+      <c r="L24" s="5">
+        <f>I18*K24</f>
+        <v>5.8946644042105278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>86</v>
       </c>
@@ -17293,20 +17428,43 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="5">
+        <f>K24-K23</f>
+        <v>-1.2069999999999997E-2</v>
+      </c>
+      <c r="L25" s="5">
+        <f>1000-(L23+L24)</f>
+        <v>987.31967649684213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="8">
+        <f>2*PI()*I16</f>
+        <v>30.457121515229453</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="5">
-        <f>L23/(I14*L24)</f>
-        <v>0.80480956192941222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="5">
+        <f>L25/I14</f>
+        <v>24.682991912421052</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f>L27/L26</f>
+        <v>0.81041775074111433</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -17315,7 +17473,7 @@
         <v>69.584399933743413</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -17326,8 +17484,20 @@
       <c r="C30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30">
+        <v>70</v>
+      </c>
+      <c r="G30" t="s">
+        <v>41</v>
+      </c>
+      <c r="K30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -17338,8 +17508,18 @@
       <c r="C31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31">
+        <f>0.064736*F30</f>
+        <v>4.5315200000000004</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -17350,8 +17530,17 @@
       <c r="C32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
@@ -17362,8 +17551,17 @@
       <c r="C33" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -17375,7 +17573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -17386,8 +17584,20 @@
       <c r="C35" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" t="s">
+        <v>132</v>
+      </c>
+      <c r="J35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -17398,11 +17608,75 @@
       <c r="C36" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>127</v>
+      </c>
+      <c r="I36">
+        <f>F32-F31</f>
+        <v>995.46848</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <f>F31/F32*100</f>
+        <v>0.45315200000000005</v>
+      </c>
+      <c r="G37" t="s">
+        <v>128</v>
+      </c>
+      <c r="I37">
+        <f>I36/(B35*B15)</f>
+        <v>0.84160178272502428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>0.066495*1100</f>
         <v>73.144499999999994</v>
+      </c>
+      <c r="E40" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40">
+        <f>0.092*70</f>
+        <v>6.4399999999999995</v>
+      </c>
+      <c r="I40">
+        <f>F32-F40-F41</f>
+        <v>987.95999999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41">
+        <f>0.08*70</f>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="I41">
+        <f>I40/(B35*B15)</f>
+        <v>0.83525386686378544</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42">
+        <f>(F41+F40)/F32*100</f>
+        <v>1.204</v>
+      </c>
+      <c r="G42" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>